<commit_message>
new data for prediction
</commit_message>
<xml_diff>
--- a/data/Served Meal Count.xlsx
+++ b/data/Served Meal Count.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Maywood-Garfield" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Maywood-Garfield'!$B$1:$B$1007</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Maywood-Garfield'!$B$1:$B$996</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -437,11 +437,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1007"/>
+  <dimension ref="A1:E996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A248" sqref="A248:XFD248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4564,15 +4564,9 @@
         <f t="shared" si="5"/>
         <v>Saturday</v>
       </c>
-      <c r="C229" s="14">
-        <v>0</v>
-      </c>
-      <c r="D229" s="14">
-        <v>0</v>
-      </c>
-      <c r="E229" s="14">
-        <v>0</v>
-      </c>
+      <c r="C229" s="14"/>
+      <c r="D229" s="14"/>
+      <c r="E229" s="14"/>
     </row>
     <row r="230" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="9">
@@ -4582,15 +4576,9 @@
         <f t="shared" si="5"/>
         <v>Sunday</v>
       </c>
-      <c r="C230" s="14">
-        <v>0</v>
-      </c>
-      <c r="D230" s="14">
-        <v>0</v>
-      </c>
-      <c r="E230" s="14">
-        <v>0</v>
-      </c>
+      <c r="C230" s="14"/>
+      <c r="D230" s="14"/>
+      <c r="E230" s="14"/>
     </row>
     <row r="231" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="9">
@@ -4690,15 +4678,9 @@
         <f t="shared" si="5"/>
         <v>Saturday</v>
       </c>
-      <c r="C236" s="14">
-        <v>0</v>
-      </c>
-      <c r="D236" s="14">
-        <v>0</v>
-      </c>
-      <c r="E236" s="14">
-        <v>0</v>
-      </c>
+      <c r="C236" s="14"/>
+      <c r="D236" s="14"/>
+      <c r="E236" s="14"/>
     </row>
     <row r="237" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="9">
@@ -4708,15 +4690,9 @@
         <f t="shared" si="5"/>
         <v>Sunday</v>
       </c>
-      <c r="C237" s="14">
-        <v>0</v>
-      </c>
-      <c r="D237" s="14">
-        <v>0</v>
-      </c>
-      <c r="E237" s="14">
-        <v>0</v>
-      </c>
+      <c r="C237" s="14"/>
+      <c r="D237" s="14"/>
+      <c r="E237" s="14"/>
     </row>
     <row r="238" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="9">
@@ -4888,15 +4864,9 @@
         <f t="shared" si="6"/>
         <v>Saturday</v>
       </c>
-      <c r="C247" s="18">
-        <v>30</v>
-      </c>
-      <c r="D247" s="18">
-        <v>33</v>
-      </c>
-      <c r="E247" s="18">
-        <v>0</v>
-      </c>
+      <c r="C247" s="18"/>
+      <c r="D247" s="18"/>
+      <c r="E247" s="18"/>
     </row>
     <row r="248" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="9">
@@ -4906,15 +4876,9 @@
         <f t="shared" si="6"/>
         <v>Sunday</v>
       </c>
-      <c r="C248" s="18">
-        <v>31</v>
-      </c>
-      <c r="D248" s="18">
-        <v>32</v>
-      </c>
-      <c r="E248" s="18">
-        <v>0</v>
-      </c>
+      <c r="C248" s="18"/>
+      <c r="D248" s="18"/>
+      <c r="E248" s="18"/>
     </row>
     <row r="249" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="9">
@@ -4997,10 +4961,10 @@
         <v>Friday</v>
       </c>
       <c r="C253" s="18">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D253" s="18">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="E253" s="18">
         <v>0</v>
@@ -5014,15 +4978,9 @@
         <f t="shared" si="6"/>
         <v>Saturday</v>
       </c>
-      <c r="C254" s="18">
-        <v>30</v>
-      </c>
-      <c r="D254" s="18">
-        <v>35</v>
-      </c>
-      <c r="E254" s="18">
-        <v>0</v>
-      </c>
+      <c r="C254" s="18"/>
+      <c r="D254" s="18"/>
+      <c r="E254" s="18"/>
     </row>
     <row r="255" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="9">
@@ -5032,15 +4990,9 @@
         <f t="shared" si="6"/>
         <v>Sunday</v>
       </c>
-      <c r="C255" s="18">
-        <v>40</v>
-      </c>
-      <c r="D255" s="18">
-        <v>36</v>
-      </c>
-      <c r="E255" s="18">
-        <v>0</v>
-      </c>
+      <c r="C255" s="18"/>
+      <c r="D255" s="18"/>
+      <c r="E255" s="18"/>
     </row>
     <row r="256" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="9">
@@ -5051,10 +5003,10 @@
         <v>Monday</v>
       </c>
       <c r="C256" s="18">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D256" s="18">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="E256" s="18">
         <v>0</v>
@@ -5065,216 +5017,73 @@
         <v>45524</v>
       </c>
       <c r="B257" s="5" t="str">
-        <f t="shared" ref="B257:B266" si="7">TEXT(A257, "dddd")</f>
+        <f t="shared" ref="B257" si="7">TEXT(A257, "dddd")</f>
         <v>Tuesday</v>
       </c>
       <c r="C257" s="18">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D257" s="18">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="E257" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A258" s="9">
-        <v>45525</v>
-      </c>
-      <c r="B258" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="C258" s="18">
-        <v>35</v>
-      </c>
-      <c r="D258" s="18">
-        <v>40</v>
-      </c>
-      <c r="E258" s="18">
-        <v>0</v>
-      </c>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+      <c r="E258" s="2"/>
     </row>
     <row r="259" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="9">
-        <v>45526</v>
-      </c>
-      <c r="B259" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Thursday</v>
-      </c>
-      <c r="C259" s="18">
-        <v>41</v>
-      </c>
-      <c r="D259" s="18">
-        <v>45</v>
-      </c>
-      <c r="E259" s="18">
-        <v>0</v>
-      </c>
+      <c r="C259" s="2"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="2"/>
     </row>
     <row r="260" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="9">
-        <v>45527</v>
-      </c>
-      <c r="B260" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Friday</v>
-      </c>
-      <c r="C260" s="18">
-        <v>40</v>
-      </c>
-      <c r="D260" s="18">
-        <v>41</v>
-      </c>
-      <c r="E260" s="18">
-        <v>0</v>
-      </c>
+      <c r="C260" s="2"/>
+      <c r="D260" s="2"/>
+      <c r="E260" s="2"/>
     </row>
     <row r="261" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="9">
-        <v>45528</v>
-      </c>
-      <c r="B261" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Saturday</v>
-      </c>
-      <c r="C261" s="18">
-        <v>42</v>
-      </c>
-      <c r="D261" s="18">
-        <v>45</v>
-      </c>
-      <c r="E261" s="18">
-        <v>0</v>
-      </c>
+      <c r="C261" s="2"/>
+      <c r="D261" s="2"/>
+      <c r="E261" s="2"/>
     </row>
     <row r="262" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A262" s="9">
-        <v>45529</v>
-      </c>
-      <c r="B262" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Sunday</v>
-      </c>
-      <c r="C262" s="18">
-        <v>39</v>
-      </c>
-      <c r="D262" s="18">
-        <v>40</v>
-      </c>
-      <c r="E262" s="18">
-        <v>0</v>
-      </c>
+      <c r="C262" s="2"/>
+      <c r="D262" s="2"/>
+      <c r="E262" s="2"/>
     </row>
     <row r="263" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A263" s="9">
-        <v>45530</v>
-      </c>
-      <c r="B263" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Monday</v>
-      </c>
-      <c r="C263" s="18">
-        <v>65</v>
-      </c>
-      <c r="D263" s="18">
-        <v>77</v>
-      </c>
-      <c r="E263" s="18">
-        <v>0</v>
-      </c>
+      <c r="C263" s="2"/>
+      <c r="D263" s="2"/>
+      <c r="E263" s="2"/>
     </row>
     <row r="264" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="9">
-        <v>45531</v>
-      </c>
-      <c r="B264" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="C264" s="18">
-        <v>66</v>
-      </c>
-      <c r="D264" s="18">
-        <v>80</v>
-      </c>
-      <c r="E264" s="18">
-        <v>0</v>
-      </c>
+      <c r="C264" s="2"/>
+      <c r="D264" s="2"/>
+      <c r="E264" s="2"/>
     </row>
     <row r="265" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="9">
-        <v>45532</v>
-      </c>
-      <c r="B265" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="C265" s="18">
-        <v>70</v>
-      </c>
-      <c r="D265" s="18">
-        <v>72</v>
-      </c>
-      <c r="E265" s="18">
-        <v>0</v>
-      </c>
+      <c r="C265" s="2"/>
+      <c r="D265" s="2"/>
+      <c r="E265" s="2"/>
     </row>
     <row r="266" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A266" s="9">
-        <v>45533</v>
-      </c>
-      <c r="B266" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Thursday</v>
-      </c>
-      <c r="C266" s="18">
-        <v>71</v>
-      </c>
-      <c r="D266" s="18">
-        <v>75</v>
-      </c>
-      <c r="E266" s="18">
-        <v>0</v>
-      </c>
+      <c r="C266" s="2"/>
+      <c r="D266" s="2"/>
+      <c r="E266" s="2"/>
     </row>
     <row r="267" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="9">
-        <v>45534</v>
-      </c>
-      <c r="B267" s="5" t="str">
-        <f>TEXT(A267, "dddd")</f>
-        <v>Friday</v>
-      </c>
-      <c r="C267" s="18">
-        <v>68</v>
-      </c>
-      <c r="D267" s="18">
-        <v>75</v>
-      </c>
-      <c r="E267" s="18">
-        <v>0</v>
-      </c>
+      <c r="C267" s="2"/>
+      <c r="D267" s="2"/>
+      <c r="E267" s="2"/>
     </row>
     <row r="268" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="9">
-        <v>45535</v>
-      </c>
-      <c r="B268" s="5" t="str">
-        <f>TEXT(A268, "dddd")</f>
-        <v>Saturday</v>
-      </c>
-      <c r="C268" s="18">
-        <v>75</v>
-      </c>
-      <c r="D268" s="18">
-        <v>78</v>
-      </c>
-      <c r="E268" s="18">
-        <v>0</v>
-      </c>
+      <c r="C268" s="2"/>
+      <c r="D268" s="2"/>
+      <c r="E268" s="2"/>
     </row>
     <row r="269" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C269" s="2"/>
@@ -8916,65 +8725,10 @@
       <c r="D996" s="2"/>
       <c r="E996" s="2"/>
     </row>
-    <row r="997" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C997" s="2"/>
-      <c r="D997" s="2"/>
-      <c r="E997" s="2"/>
-    </row>
-    <row r="998" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C998" s="2"/>
-      <c r="D998" s="2"/>
-      <c r="E998" s="2"/>
-    </row>
-    <row r="999" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-    </row>
-    <row r="1000" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-    </row>
-    <row r="1001" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1001" s="2"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="2"/>
-    </row>
-    <row r="1002" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1002" s="2"/>
-      <c r="D1002" s="2"/>
-      <c r="E1002" s="2"/>
-    </row>
-    <row r="1003" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1003" s="2"/>
-      <c r="D1003" s="2"/>
-      <c r="E1003" s="2"/>
-    </row>
-    <row r="1004" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1004" s="2"/>
-      <c r="D1004" s="2"/>
-      <c r="E1004" s="2"/>
-    </row>
-    <row r="1005" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1005" s="2"/>
-      <c r="D1005" s="2"/>
-      <c r="E1005" s="2"/>
-    </row>
-    <row r="1006" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1006" s="2"/>
-      <c r="D1006" s="2"/>
-      <c r="E1006" s="2"/>
-    </row>
-    <row r="1007" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1007" s="2"/>
-      <c r="D1007" s="2"/>
-      <c r="E1007" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:B1007"/>
+  <autoFilter ref="B1:B996"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>